<commit_message>
Sprint 2 INSERT klant
</commit_message>
<xml_diff>
--- a/Requirements and Planning/burndown_Bas-1.xlsx
+++ b/Requirements and Planning/burndown_Bas-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Project_Bas\Requirements and Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1924EF-B6B2-46AC-9823-2F5B8BCFBDE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D6B9AB7-8F56-4CAD-B03D-23E1BCD5AB4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{D64FC014-072E-4862-83BE-4A77B874CE33}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>Taak</t>
   </si>
@@ -624,19 +624,19 @@
                   <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>51</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>51</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>51</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>51</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>51</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1917,7 +1917,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2128,9 +2128,7 @@
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -2145,9 +2143,7 @@
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -2162,8 +2158,8 @@
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="2" t="s">
-        <v>18</v>
+      <c r="E13" s="2">
+        <v>6</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -2281,7 +2277,9 @@
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="E20" s="2">
+        <v>2</v>
+      </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2" t="s">
@@ -2360,23 +2358,23 @@
       </c>
       <c r="E24" s="9">
         <f t="shared" ref="E24:I24" si="0">D$24-SUM(E3:E23)</f>
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="F24" s="9">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G24" s="9">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="H24" s="9">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="I24" s="10">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>